<commit_message>
add function to save timer_count - it need for tuning time.sleep(interval)
</commit_message>
<xml_diff>
--- a/df_help_06.03.2022.xlsx
+++ b/df_help_06.03.2022.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="135">
   <si>
     <t>краткое наименование инструмента</t>
   </si>
@@ -128,54 +128,6 @@
     <t>today_close</t>
   </si>
   <si>
-    <t>mean_min_dek1</t>
-  </si>
-  <si>
-    <t>mean_min_dek2</t>
-  </si>
-  <si>
-    <t>mean_min_dek3</t>
-  </si>
-  <si>
-    <t>mean_min_dek4</t>
-  </si>
-  <si>
-    <t>mean_min_dek5</t>
-  </si>
-  <si>
-    <t>mean_min_dek6</t>
-  </si>
-  <si>
-    <t>mean_min_dek7</t>
-  </si>
-  <si>
-    <t>mean_min_dek8</t>
-  </si>
-  <si>
-    <t>mean_min_pr_dek1</t>
-  </si>
-  <si>
-    <t>mean_min_pr_dek2</t>
-  </si>
-  <si>
-    <t>mean_min_pr_dek3</t>
-  </si>
-  <si>
-    <t>mean_min_pr_dek4</t>
-  </si>
-  <si>
-    <t>mean_min_pr_dek5</t>
-  </si>
-  <si>
-    <t>mean_min_pr_dek6</t>
-  </si>
-  <si>
-    <t>mean_min_pr_dek7</t>
-  </si>
-  <si>
-    <t>mean_min_pr_dek8</t>
-  </si>
-  <si>
     <t>min_pr_delta_1_2</t>
   </si>
   <si>
@@ -330,9 +282,6 @@
   </si>
   <si>
     <t>минимальная  стоимость среди дневных минимальных за период</t>
-  </si>
-  <si>
-    <t>min_min_dek1</t>
   </si>
   <si>
     <t>branch</t>
@@ -522,6 +471,54 @@
   </si>
   <si>
     <t xml:space="preserve">максимальная стоимость среди дневных максимальных за период </t>
+  </si>
+  <si>
+    <t>min_dek2</t>
+  </si>
+  <si>
+    <t>min_dek3</t>
+  </si>
+  <si>
+    <t>min_dek4</t>
+  </si>
+  <si>
+    <t>min_dek5</t>
+  </si>
+  <si>
+    <t>min_dek6</t>
+  </si>
+  <si>
+    <t>min_dek7</t>
+  </si>
+  <si>
+    <t>min_dek8</t>
+  </si>
+  <si>
+    <t>min_dek1</t>
+  </si>
+  <si>
+    <t>min_pr_dek1</t>
+  </si>
+  <si>
+    <t>min_pr_dek2</t>
+  </si>
+  <si>
+    <t>min_pr_dek3</t>
+  </si>
+  <si>
+    <t>min_pr_dek4</t>
+  </si>
+  <si>
+    <t>min_pr_dek5</t>
+  </si>
+  <si>
+    <t>min_pr_dek6</t>
+  </si>
+  <si>
+    <t>min_pr_dek7</t>
+  </si>
+  <si>
+    <t>min_pr_dek8</t>
   </si>
 </sst>
 </file>
@@ -894,22 +891,31 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -921,12 +927,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -936,13 +936,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -951,23 +954,17 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1200,7 +1197,7 @@
   <dimension ref="B1:CI6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1"/>
@@ -1225,19 +1222,19 @@
         <v>1</v>
       </c>
       <c r="D1" s="2"/>
-      <c r="E1" s="34" t="s">
-        <v>105</v>
-      </c>
-      <c r="F1" s="43" t="s">
-        <v>101</v>
-      </c>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
+      <c r="E1" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
       <c r="N1" s="33" t="s">
         <v>2</v>
       </c>
@@ -1257,16 +1254,16 @@
       <c r="Z1" s="33"/>
       <c r="AA1" s="33"/>
       <c r="AB1" s="33"/>
-      <c r="AC1" s="45" t="s">
-        <v>135</v>
-      </c>
-      <c r="AD1" s="45"/>
-      <c r="AE1" s="45"/>
-      <c r="AF1" s="45"/>
-      <c r="AG1" s="45"/>
-      <c r="AH1" s="45"/>
-      <c r="AI1" s="45"/>
-      <c r="AJ1" s="45"/>
+      <c r="AC1" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD1" s="34"/>
+      <c r="AE1" s="34"/>
+      <c r="AF1" s="34"/>
+      <c r="AG1" s="34"/>
+      <c r="AH1" s="34"/>
+      <c r="AI1" s="34"/>
+      <c r="AJ1" s="34"/>
       <c r="AK1" s="33" t="s">
         <v>4</v>
       </c>
@@ -1286,7 +1283,7 @@
       <c r="AW1" s="33"/>
       <c r="AX1" s="33"/>
       <c r="AY1" s="33"/>
-      <c r="AZ1" s="46" t="s">
+      <c r="AZ1" s="36" t="s">
         <v>5</v>
       </c>
       <c r="BA1" s="35" t="s">
@@ -1309,17 +1306,17 @@
       <c r="B2" s="35"/>
       <c r="C2" s="35"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="36" t="s">
-        <v>110</v>
-      </c>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="41"/>
       <c r="N2" s="33" t="s">
         <v>11</v>
       </c>
@@ -1339,16 +1336,16 @@
       <c r="Z2" s="33"/>
       <c r="AA2" s="33"/>
       <c r="AB2" s="33"/>
-      <c r="AC2" s="36" t="s">
-        <v>110</v>
-      </c>
-      <c r="AD2" s="37"/>
-      <c r="AE2" s="37"/>
-      <c r="AF2" s="37"/>
-      <c r="AG2" s="37"/>
-      <c r="AH2" s="37"/>
-      <c r="AI2" s="37"/>
-      <c r="AJ2" s="38"/>
+      <c r="AC2" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="AD2" s="40"/>
+      <c r="AE2" s="40"/>
+      <c r="AF2" s="40"/>
+      <c r="AG2" s="40"/>
+      <c r="AH2" s="40"/>
+      <c r="AI2" s="40"/>
+      <c r="AJ2" s="41"/>
       <c r="AK2" s="33" t="s">
         <v>13</v>
       </c>
@@ -1368,7 +1365,7 @@
       <c r="AW2" s="33"/>
       <c r="AX2" s="33"/>
       <c r="AY2" s="33"/>
-      <c r="AZ2" s="46"/>
+      <c r="AZ2" s="36"/>
       <c r="BA2" s="35"/>
       <c r="BB2" s="35"/>
       <c r="BC2" s="35"/>
@@ -1382,33 +1379,33 @@
       <c r="BY2"/>
       <c r="BZ2"/>
       <c r="CA2"/>
-      <c r="CB2" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="CC2" s="30"/>
-      <c r="CD2" s="30"/>
-      <c r="CE2" s="30"/>
-      <c r="CF2" s="30"/>
-      <c r="CG2" s="30"/>
-      <c r="CH2" s="30"/>
-      <c r="CI2" s="30"/>
+      <c r="CB2" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="CC2" s="45"/>
+      <c r="CD2" s="45"/>
+      <c r="CE2" s="45"/>
+      <c r="CF2" s="45"/>
+      <c r="CG2" s="45"/>
+      <c r="CH2" s="45"/>
+      <c r="CI2" s="45"/>
     </row>
     <row r="3" spans="2:87" s="1" customFormat="1" ht="31.5" customHeight="1" thickBot="1">
       <c r="B3" s="35"/>
       <c r="C3" s="35"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="34"/>
+      <c r="E3" s="38"/>
       <c r="F3" s="5" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>16</v>
@@ -1423,16 +1420,16 @@
         <v>19</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="R3" s="5" t="s">
         <v>16</v>
@@ -1454,16 +1451,16 @@
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
       <c r="AC3" s="5" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="AD3" s="5" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="AE3" s="5" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="AF3" s="5" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="AG3" s="5" t="s">
         <v>16</v>
@@ -1478,16 +1475,16 @@
         <v>19</v>
       </c>
       <c r="AK3" s="5" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="AL3" s="5" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="AM3" s="5" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="AN3" s="5" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="AO3" s="5" t="s">
         <v>16</v>
@@ -1508,50 +1505,50 @@
       <c r="AW3" s="17"/>
       <c r="AX3" s="17"/>
       <c r="AY3" s="17"/>
-      <c r="AZ3" s="46"/>
+      <c r="AZ3" s="36"/>
       <c r="BA3" s="35"/>
       <c r="BB3" s="35"/>
       <c r="BC3" s="35"/>
       <c r="BD3" s="4"/>
       <c r="BE3" s="4"/>
-      <c r="BT3" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="BU3" s="31"/>
-      <c r="BV3" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="BW3" s="31"/>
-      <c r="BX3" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="BY3" s="31"/>
-      <c r="BZ3" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="CA3" s="31"/>
-      <c r="CB3" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="CC3" s="31"/>
-      <c r="CD3" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="CE3" s="31"/>
-      <c r="CF3" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="CG3" s="31"/>
-      <c r="CH3" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="CI3" s="31"/>
+      <c r="BT3" s="46" t="s">
+        <v>113</v>
+      </c>
+      <c r="BU3" s="46"/>
+      <c r="BV3" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="BW3" s="46"/>
+      <c r="BX3" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="BY3" s="46"/>
+      <c r="BZ3" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="CA3" s="46"/>
+      <c r="CB3" s="46" t="s">
+        <v>113</v>
+      </c>
+      <c r="CC3" s="46"/>
+      <c r="CD3" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="CE3" s="46"/>
+      <c r="CF3" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="CG3" s="46"/>
+      <c r="CH3" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="CI3" s="46"/>
     </row>
     <row r="4" spans="2:87" s="1" customFormat="1" ht="48" customHeight="1" thickBot="1">
       <c r="B4" s="35"/>
       <c r="C4" s="35"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="34"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="18"/>
       <c r="G4" s="18"/>
       <c r="H4" s="18"/>
@@ -1560,25 +1557,25 @@
       <c r="K4" s="18"/>
       <c r="L4" s="18"/>
       <c r="M4" s="18"/>
-      <c r="N4" s="39" t="s">
+      <c r="N4" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="O4" s="39"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="39"/>
-      <c r="S4" s="39"/>
-      <c r="T4" s="39"/>
-      <c r="U4" s="39"/>
-      <c r="V4" s="40" t="s">
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="30"/>
+      <c r="U4" s="30"/>
+      <c r="V4" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="W4" s="40"/>
-      <c r="X4" s="40"/>
-      <c r="Y4" s="40"/>
-      <c r="Z4" s="40"/>
-      <c r="AA4" s="40"/>
-      <c r="AB4" s="40"/>
+      <c r="W4" s="31"/>
+      <c r="X4" s="31"/>
+      <c r="Y4" s="31"/>
+      <c r="Z4" s="31"/>
+      <c r="AA4" s="31"/>
+      <c r="AB4" s="31"/>
       <c r="AC4" s="18"/>
       <c r="AD4" s="18"/>
       <c r="AE4" s="18"/>
@@ -1587,51 +1584,51 @@
       <c r="AH4" s="18"/>
       <c r="AI4" s="18"/>
       <c r="AJ4" s="18"/>
-      <c r="AK4" s="39" t="s">
+      <c r="AK4" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="AL4" s="39"/>
-      <c r="AM4" s="39"/>
-      <c r="AN4" s="39"/>
-      <c r="AO4" s="39"/>
-      <c r="AP4" s="39"/>
-      <c r="AQ4" s="39"/>
-      <c r="AR4" s="39"/>
-      <c r="AS4" s="40" t="s">
+      <c r="AL4" s="30"/>
+      <c r="AM4" s="30"/>
+      <c r="AN4" s="30"/>
+      <c r="AO4" s="30"/>
+      <c r="AP4" s="30"/>
+      <c r="AQ4" s="30"/>
+      <c r="AR4" s="30"/>
+      <c r="AS4" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="AT4" s="40"/>
-      <c r="AU4" s="40"/>
-      <c r="AV4" s="40"/>
-      <c r="AW4" s="40"/>
-      <c r="AX4" s="40"/>
-      <c r="AY4" s="40"/>
+      <c r="AT4" s="31"/>
+      <c r="AU4" s="31"/>
+      <c r="AV4" s="31"/>
+      <c r="AW4" s="31"/>
+      <c r="AX4" s="31"/>
+      <c r="AY4" s="31"/>
       <c r="AZ4" s="7"/>
       <c r="BA4" s="7"/>
-      <c r="BB4" s="44" t="s">
+      <c r="BB4" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="BC4" s="44"/>
+      <c r="BC4" s="32"/>
       <c r="BD4" s="4"/>
       <c r="BE4" s="4"/>
-      <c r="BF4" s="41" t="s">
-        <v>100</v>
-      </c>
-      <c r="BG4" s="42"/>
-      <c r="BH4" s="42"/>
-      <c r="BI4" s="42"/>
-      <c r="BJ4" s="42"/>
-      <c r="BK4" s="42"/>
-      <c r="BL4" s="42"/>
-      <c r="BM4" s="42"/>
-      <c r="BN4" s="42"/>
-      <c r="BO4" s="42"/>
-      <c r="BP4" s="42"/>
-      <c r="BQ4" s="42"/>
-      <c r="BR4" s="42"/>
-      <c r="BS4" s="42"/>
-      <c r="BT4" s="32" t="s">
-        <v>129</v>
+      <c r="BF4" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="BG4" s="43"/>
+      <c r="BH4" s="43"/>
+      <c r="BI4" s="43"/>
+      <c r="BJ4" s="43"/>
+      <c r="BK4" s="43"/>
+      <c r="BL4" s="43"/>
+      <c r="BM4" s="43"/>
+      <c r="BN4" s="43"/>
+      <c r="BO4" s="43"/>
+      <c r="BP4" s="43"/>
+      <c r="BQ4" s="43"/>
+      <c r="BR4" s="43"/>
+      <c r="BS4" s="43"/>
+      <c r="BT4" s="37" t="s">
+        <v>112</v>
       </c>
       <c r="BU4" s="33"/>
       <c r="BV4" s="33"/>
@@ -1651,7 +1648,7 @@
     </row>
     <row r="5" spans="2:87" s="1" customFormat="1" ht="22.5" customHeight="1">
       <c r="D5" s="15" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="F5" s="18">
         <v>1</v>
@@ -1788,270 +1785,269 @@
         <v>32</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>33</v>
       </c>
       <c r="F6" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="L6" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="M6" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="N6" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="O6" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="P6" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q6" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="R6" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="S6" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="T6" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="U6" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="V6" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="W6" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="X6" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y6" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z6" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA6" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB6" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC6" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD6" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE6" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF6" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG6" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="AH6" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI6" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ6" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK6" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="AL6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM6" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="AN6" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="AO6" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP6" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ6" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="AR6" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS6" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="AT6" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU6" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="AV6" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="AW6" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="AX6" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="AY6" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="AZ6" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="BA6" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="BB6" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BC6" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="BD6" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="BE6" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="BF6" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="BG6" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="BH6" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="BI6" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="BJ6" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="BK6" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="BL6" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="BM6" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="BN6" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="BO6" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="BP6" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="BQ6" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="BR6" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="BS6" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="BT6" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="BU6" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="BV6" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="BW6" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="BX6" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="BY6" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="BZ6" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="G6" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="I6" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="J6" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="K6" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="L6" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="M6" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="N6" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="O6" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="P6" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q6" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="R6" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="S6" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="T6" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="U6" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="V6" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="W6" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="X6" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y6" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="Z6" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA6" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB6" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="AC6" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD6" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE6" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF6" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="AG6" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="AH6" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="AI6" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="AJ6" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="AK6" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="AL6" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="AM6" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="AN6" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="AO6" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="AP6" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="AQ6" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="AR6" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="AS6" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="AT6" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="AU6" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="AV6" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="AW6" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="AX6" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="AY6" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="AZ6" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="BA6" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="BB6" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="BC6" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="BD6" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="BE6" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="BF6" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="BG6" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="BH6" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="BI6" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="BJ6" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="BK6" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL6" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="BM6" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="BN6" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="BO6" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="BP6" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="BQ6" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="BR6" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="BS6" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="BT6" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="BU6" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="BV6" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="BW6" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="BX6" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="BY6" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="BZ6" s="25" t="s">
-        <v>119</v>
-      </c>
       <c r="CA6" s="25" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="CB6" s="24" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="CC6" s="14" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="CD6" s="14" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="CE6" s="14" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="CF6" s="14" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="CG6" s="14" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="CH6" s="14" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="CI6" s="14" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="AK4:AR4"/>
-    <mergeCell ref="AS4:AY4"/>
-    <mergeCell ref="BB4:BC4"/>
-    <mergeCell ref="V1:AB1"/>
-    <mergeCell ref="AC1:AJ1"/>
-    <mergeCell ref="AK1:AR1"/>
-    <mergeCell ref="BC1:BC3"/>
-    <mergeCell ref="AZ1:AZ3"/>
-    <mergeCell ref="BA1:BA3"/>
-    <mergeCell ref="BB1:BB3"/>
+    <mergeCell ref="CB2:CI2"/>
+    <mergeCell ref="BT3:BU3"/>
+    <mergeCell ref="BV3:BW3"/>
+    <mergeCell ref="BX3:BY3"/>
+    <mergeCell ref="BZ3:CA3"/>
+    <mergeCell ref="CB3:CC3"/>
+    <mergeCell ref="CD3:CE3"/>
+    <mergeCell ref="CF3:CG3"/>
+    <mergeCell ref="CH3:CI3"/>
     <mergeCell ref="BT4:CI4"/>
     <mergeCell ref="AS1:AY1"/>
     <mergeCell ref="N2:U2"/>
@@ -2068,15 +2064,16 @@
     <mergeCell ref="AS2:AY2"/>
     <mergeCell ref="F1:M1"/>
     <mergeCell ref="N1:U1"/>
-    <mergeCell ref="CB2:CI2"/>
-    <mergeCell ref="BT3:BU3"/>
-    <mergeCell ref="BV3:BW3"/>
-    <mergeCell ref="BX3:BY3"/>
-    <mergeCell ref="BZ3:CA3"/>
-    <mergeCell ref="CB3:CC3"/>
-    <mergeCell ref="CD3:CE3"/>
-    <mergeCell ref="CF3:CG3"/>
-    <mergeCell ref="CH3:CI3"/>
+    <mergeCell ref="AK4:AR4"/>
+    <mergeCell ref="AS4:AY4"/>
+    <mergeCell ref="BB4:BC4"/>
+    <mergeCell ref="V1:AB1"/>
+    <mergeCell ref="AC1:AJ1"/>
+    <mergeCell ref="AK1:AR1"/>
+    <mergeCell ref="BC1:BC3"/>
+    <mergeCell ref="AZ1:AZ3"/>
+    <mergeCell ref="BA1:BA3"/>
+    <mergeCell ref="BB1:BB3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2088,7 +2085,7 @@
   <dimension ref="A1:CI6"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AC1" sqref="AC1:AJ1"/>
+      <selection activeCell="F6" sqref="F6:U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1"/>
@@ -2102,26 +2099,26 @@
   <sheetData>
     <row r="1" spans="1:87" ht="51.75" customHeight="1">
       <c r="A1" s="2"/>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="47" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="35" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2"/>
-      <c r="E1" s="34" t="s">
-        <v>105</v>
-      </c>
-      <c r="F1" s="50" t="s">
-        <v>101</v>
-      </c>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
+      <c r="E1" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
       <c r="N1" s="35" t="s">
         <v>2</v>
       </c>
@@ -2141,16 +2138,16 @@
       <c r="Z1" s="35"/>
       <c r="AA1" s="35"/>
       <c r="AB1" s="35"/>
-      <c r="AC1" s="45" t="s">
-        <v>135</v>
-      </c>
-      <c r="AD1" s="45"/>
-      <c r="AE1" s="45"/>
-      <c r="AF1" s="45"/>
-      <c r="AG1" s="45"/>
-      <c r="AH1" s="45"/>
-      <c r="AI1" s="45"/>
-      <c r="AJ1" s="45"/>
+      <c r="AC1" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD1" s="34"/>
+      <c r="AE1" s="34"/>
+      <c r="AF1" s="34"/>
+      <c r="AG1" s="34"/>
+      <c r="AH1" s="34"/>
+      <c r="AI1" s="34"/>
+      <c r="AJ1" s="34"/>
       <c r="AK1" s="35" t="s">
         <v>4</v>
       </c>
@@ -2191,20 +2188,20 @@
     </row>
     <row r="2" spans="1:87">
       <c r="A2" s="2"/>
-      <c r="B2" s="49"/>
+      <c r="B2" s="47"/>
       <c r="C2" s="35"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="36" t="s">
-        <v>110</v>
-      </c>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="41"/>
       <c r="N2" s="35" t="s">
         <v>11</v>
       </c>
@@ -2224,16 +2221,16 @@
       <c r="Z2" s="35"/>
       <c r="AA2" s="35"/>
       <c r="AB2" s="35"/>
-      <c r="AC2" s="36" t="s">
-        <v>110</v>
-      </c>
-      <c r="AD2" s="37"/>
-      <c r="AE2" s="37"/>
-      <c r="AF2" s="37"/>
-      <c r="AG2" s="37"/>
-      <c r="AH2" s="37"/>
-      <c r="AI2" s="37"/>
-      <c r="AJ2" s="38"/>
+      <c r="AC2" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="AD2" s="40"/>
+      <c r="AE2" s="40"/>
+      <c r="AF2" s="40"/>
+      <c r="AG2" s="40"/>
+      <c r="AH2" s="40"/>
+      <c r="AI2" s="40"/>
+      <c r="AJ2" s="41"/>
       <c r="AK2" s="35" t="s">
         <v>13</v>
       </c>
@@ -2259,34 +2256,34 @@
       <c r="BC2" s="35"/>
       <c r="BD2" s="4"/>
       <c r="BE2" s="4"/>
-      <c r="CB2" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="CC2" s="30"/>
-      <c r="CD2" s="30"/>
-      <c r="CE2" s="30"/>
-      <c r="CF2" s="30"/>
-      <c r="CG2" s="30"/>
-      <c r="CH2" s="30"/>
-      <c r="CI2" s="30"/>
+      <c r="CB2" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="CC2" s="45"/>
+      <c r="CD2" s="45"/>
+      <c r="CE2" s="45"/>
+      <c r="CF2" s="45"/>
+      <c r="CG2" s="45"/>
+      <c r="CH2" s="45"/>
+      <c r="CI2" s="45"/>
     </row>
     <row r="3" spans="1:87" ht="30.75" customHeight="1" thickBot="1">
       <c r="A3" s="2"/>
-      <c r="B3" s="49"/>
+      <c r="B3" s="47"/>
       <c r="C3" s="35"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="34"/>
+      <c r="E3" s="38"/>
       <c r="F3" s="5" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>16</v>
@@ -2301,16 +2298,16 @@
         <v>19</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="R3" s="5" t="s">
         <v>16</v>
@@ -2332,16 +2329,16 @@
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
       <c r="AC3" s="5" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="AD3" s="5" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="AE3" s="5" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="AF3" s="5" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="AG3" s="5" t="s">
         <v>16</v>
@@ -2356,16 +2353,16 @@
         <v>19</v>
       </c>
       <c r="AK3" s="5" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="AL3" s="5" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="AM3" s="5" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="AN3" s="5" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="AO3" s="5" t="s">
         <v>16</v>
@@ -2392,45 +2389,45 @@
       <c r="BC3" s="35"/>
       <c r="BD3" s="4"/>
       <c r="BE3" s="4"/>
-      <c r="BT3" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="BU3" s="31"/>
-      <c r="BV3" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="BW3" s="31"/>
-      <c r="BX3" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="BY3" s="31"/>
-      <c r="BZ3" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="CA3" s="31"/>
-      <c r="CB3" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="CC3" s="31"/>
-      <c r="CD3" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="CE3" s="31"/>
-      <c r="CF3" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="CG3" s="31"/>
-      <c r="CH3" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="CI3" s="31"/>
+      <c r="BT3" s="46" t="s">
+        <v>113</v>
+      </c>
+      <c r="BU3" s="46"/>
+      <c r="BV3" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="BW3" s="46"/>
+      <c r="BX3" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="BY3" s="46"/>
+      <c r="BZ3" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="CA3" s="46"/>
+      <c r="CB3" s="46" t="s">
+        <v>113</v>
+      </c>
+      <c r="CC3" s="46"/>
+      <c r="CD3" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="CE3" s="46"/>
+      <c r="CF3" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="CG3" s="46"/>
+      <c r="CH3" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="CI3" s="46"/>
     </row>
     <row r="4" spans="1:87" ht="35.25" customHeight="1" thickBot="1">
       <c r="A4" s="2"/>
-      <c r="B4" s="49"/>
+      <c r="B4" s="47"/>
       <c r="C4" s="35"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="34"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -2439,25 +2436,25 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
-      <c r="N4" s="47" t="s">
+      <c r="N4" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="O4" s="47"/>
-      <c r="P4" s="47"/>
-      <c r="Q4" s="47"/>
-      <c r="R4" s="47"/>
-      <c r="S4" s="47"/>
-      <c r="T4" s="47"/>
-      <c r="U4" s="47"/>
-      <c r="V4" s="48" t="s">
+      <c r="O4" s="49"/>
+      <c r="P4" s="49"/>
+      <c r="Q4" s="49"/>
+      <c r="R4" s="49"/>
+      <c r="S4" s="49"/>
+      <c r="T4" s="49"/>
+      <c r="U4" s="49"/>
+      <c r="V4" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="W4" s="48"/>
-      <c r="X4" s="48"/>
-      <c r="Y4" s="48"/>
-      <c r="Z4" s="48"/>
-      <c r="AA4" s="48"/>
-      <c r="AB4" s="48"/>
+      <c r="W4" s="50"/>
+      <c r="X4" s="50"/>
+      <c r="Y4" s="50"/>
+      <c r="Z4" s="50"/>
+      <c r="AA4" s="50"/>
+      <c r="AB4" s="50"/>
       <c r="AC4" s="5"/>
       <c r="AD4" s="5"/>
       <c r="AE4" s="5"/>
@@ -2466,51 +2463,51 @@
       <c r="AH4" s="5"/>
       <c r="AI4" s="5"/>
       <c r="AJ4" s="5"/>
-      <c r="AK4" s="47" t="s">
+      <c r="AK4" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="AL4" s="47"/>
-      <c r="AM4" s="47"/>
-      <c r="AN4" s="47"/>
-      <c r="AO4" s="47"/>
-      <c r="AP4" s="47"/>
-      <c r="AQ4" s="47"/>
-      <c r="AR4" s="47"/>
-      <c r="AS4" s="48" t="s">
+      <c r="AL4" s="49"/>
+      <c r="AM4" s="49"/>
+      <c r="AN4" s="49"/>
+      <c r="AO4" s="49"/>
+      <c r="AP4" s="49"/>
+      <c r="AQ4" s="49"/>
+      <c r="AR4" s="49"/>
+      <c r="AS4" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="AT4" s="48"/>
-      <c r="AU4" s="48"/>
-      <c r="AV4" s="48"/>
-      <c r="AW4" s="48"/>
-      <c r="AX4" s="48"/>
-      <c r="AY4" s="48"/>
+      <c r="AT4" s="50"/>
+      <c r="AU4" s="50"/>
+      <c r="AV4" s="50"/>
+      <c r="AW4" s="50"/>
+      <c r="AX4" s="50"/>
+      <c r="AY4" s="50"/>
       <c r="AZ4" s="7"/>
       <c r="BA4" s="7"/>
-      <c r="BB4" s="44" t="s">
+      <c r="BB4" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="BC4" s="44"/>
+      <c r="BC4" s="32"/>
       <c r="BD4" s="4"/>
       <c r="BE4" s="4"/>
-      <c r="BF4" s="41" t="s">
-        <v>100</v>
-      </c>
-      <c r="BG4" s="42"/>
-      <c r="BH4" s="42"/>
-      <c r="BI4" s="42"/>
-      <c r="BJ4" s="42"/>
-      <c r="BK4" s="42"/>
-      <c r="BL4" s="42"/>
-      <c r="BM4" s="42"/>
-      <c r="BN4" s="42"/>
-      <c r="BO4" s="42"/>
-      <c r="BP4" s="42"/>
-      <c r="BQ4" s="42"/>
-      <c r="BR4" s="42"/>
-      <c r="BS4" s="42"/>
-      <c r="BT4" s="32" t="s">
-        <v>129</v>
+      <c r="BF4" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="BG4" s="43"/>
+      <c r="BH4" s="43"/>
+      <c r="BI4" s="43"/>
+      <c r="BJ4" s="43"/>
+      <c r="BK4" s="43"/>
+      <c r="BL4" s="43"/>
+      <c r="BM4" s="43"/>
+      <c r="BN4" s="43"/>
+      <c r="BO4" s="43"/>
+      <c r="BP4" s="43"/>
+      <c r="BQ4" s="43"/>
+      <c r="BR4" s="43"/>
+      <c r="BS4" s="43"/>
+      <c r="BT4" s="37" t="s">
+        <v>112</v>
       </c>
       <c r="BU4" s="33"/>
       <c r="BV4" s="33"/>
@@ -2533,7 +2530,7 @@
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="15" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="5">
@@ -2687,267 +2684,272 @@
         <v>32</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>33</v>
       </c>
       <c r="F6" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="P6" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q6" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="R6" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="S6" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="T6" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="U6" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="V6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="W6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="X6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="Y6" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="Z6" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="AA6" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="AB6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="M6" s="11" t="s">
+      <c r="AC6" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="AD6" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="AE6" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="P6" s="11" t="s">
+      <c r="AF6" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="Q6" s="11" t="s">
+      <c r="AG6" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="R6" s="11" t="s">
+      <c r="AH6" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="S6" s="11" t="s">
+      <c r="AI6" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="T6" s="11" t="s">
+      <c r="AJ6" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="U6" s="11" t="s">
+      <c r="AK6" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="V6" s="11" t="s">
+      <c r="AL6" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="W6" s="11" t="s">
+      <c r="AM6" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="X6" s="11" t="s">
+      <c r="AN6" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="Y6" s="11" t="s">
+      <c r="AO6" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="Z6" s="11" t="s">
+      <c r="AP6" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="AA6" s="11" t="s">
+      <c r="AQ6" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="AB6" s="11" t="s">
+      <c r="AR6" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AC6" s="11" t="s">
+      <c r="AS6" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="AD6" s="11" t="s">
+      <c r="AT6" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="AE6" s="11" t="s">
+      <c r="AU6" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="AF6" s="11" t="s">
+      <c r="AV6" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AG6" s="11" t="s">
+      <c r="AW6" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AH6" s="11" t="s">
+      <c r="AX6" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="AI6" s="11" t="s">
+      <c r="AY6" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="AJ6" s="11" t="s">
+      <c r="AZ6" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="AK6" s="11" t="s">
+      <c r="BA6" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="AL6" s="11" t="s">
+      <c r="BB6" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="AM6" s="11" t="s">
+      <c r="BC6" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="AN6" s="11" t="s">
+      <c r="BD6" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="AO6" s="11" t="s">
+      <c r="BE6" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="AP6" s="11" t="s">
+      <c r="BF6" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="AQ6" s="11" t="s">
+      <c r="BG6" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="AR6" s="11" t="s">
+      <c r="BH6" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="AS6" s="11" t="s">
+      <c r="BI6" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="AT6" s="11" t="s">
+      <c r="BJ6" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="AU6" s="11" t="s">
+      <c r="BK6" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="AV6" s="11" t="s">
+      <c r="BL6" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="AW6" s="11" t="s">
+      <c r="BM6" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="AX6" s="11" t="s">
+      <c r="BN6" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="AY6" s="11" t="s">
+      <c r="BO6" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="AZ6" s="11" t="s">
+      <c r="BP6" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="BA6" s="11" t="s">
+      <c r="BQ6" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="BB6" s="11" t="s">
+      <c r="BR6" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="BC6" s="11" t="s">
+      <c r="BS6" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="BD6" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="BE6" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="BF6" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="BG6" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="BH6" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="BI6" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="BJ6" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="BK6" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL6" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="BM6" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="BN6" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="BO6" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="BP6" s="14" t="s">
+      <c r="BT6" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="BQ6" s="14" t="s">
+      <c r="BU6" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="BR6" s="13" t="s">
+      <c r="BV6" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="BS6" s="13" t="s">
+      <c r="BW6" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="BT6" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="BU6" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="BV6" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="BW6" s="25" t="s">
-        <v>116</v>
-      </c>
       <c r="BX6" s="25" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="BY6" s="25" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="BZ6" s="25" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="CA6" s="25" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="CB6" s="24" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="CC6" s="14" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="CD6" s="14" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="CE6" s="14" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="CF6" s="14" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="CG6" s="14" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="CH6" s="14" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="CI6" s="14" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="F2:M2"/>
-    <mergeCell ref="AK1:AR1"/>
-    <mergeCell ref="E1:E4"/>
-    <mergeCell ref="F1:M1"/>
-    <mergeCell ref="V1:AB1"/>
-    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="CH3:CI3"/>
+    <mergeCell ref="CB2:CI2"/>
+    <mergeCell ref="BV3:BW3"/>
+    <mergeCell ref="BX3:BY3"/>
+    <mergeCell ref="BZ3:CA3"/>
+    <mergeCell ref="CB3:CC3"/>
+    <mergeCell ref="CD3:CE3"/>
+    <mergeCell ref="BT3:BU3"/>
+    <mergeCell ref="AZ1:AZ3"/>
+    <mergeCell ref="BA1:BA3"/>
+    <mergeCell ref="AS1:AY1"/>
+    <mergeCell ref="CF3:CG3"/>
     <mergeCell ref="BT4:CI4"/>
     <mergeCell ref="BF4:BS4"/>
     <mergeCell ref="BB4:BC4"/>
@@ -2964,18 +2966,13 @@
     <mergeCell ref="AC2:AJ2"/>
     <mergeCell ref="AC1:AJ1"/>
     <mergeCell ref="N1:U1"/>
-    <mergeCell ref="BT3:BU3"/>
-    <mergeCell ref="AZ1:AZ3"/>
-    <mergeCell ref="BA1:BA3"/>
-    <mergeCell ref="AS1:AY1"/>
-    <mergeCell ref="CF3:CG3"/>
-    <mergeCell ref="CH3:CI3"/>
-    <mergeCell ref="CB2:CI2"/>
-    <mergeCell ref="BV3:BW3"/>
-    <mergeCell ref="BX3:BY3"/>
-    <mergeCell ref="BZ3:CA3"/>
-    <mergeCell ref="CB3:CC3"/>
-    <mergeCell ref="CD3:CE3"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="F2:M2"/>
+    <mergeCell ref="AK1:AR1"/>
+    <mergeCell ref="E1:E4"/>
+    <mergeCell ref="F1:M1"/>
+    <mergeCell ref="V1:AB1"/>
+    <mergeCell ref="C1:C4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2985,8 +2982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CI6"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AC1" sqref="AC1:AJ1"/>
+    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6:U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1"/>
@@ -3007,19 +3004,19 @@
         <v>1</v>
       </c>
       <c r="D1" s="2"/>
-      <c r="E1" s="34" t="s">
-        <v>105</v>
-      </c>
-      <c r="F1" s="50" t="s">
-        <v>101</v>
-      </c>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
+      <c r="E1" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
       <c r="N1" s="35" t="s">
         <v>2</v>
       </c>
@@ -3039,16 +3036,16 @@
       <c r="Z1" s="35"/>
       <c r="AA1" s="35"/>
       <c r="AB1" s="35"/>
-      <c r="AC1" s="45" t="s">
-        <v>135</v>
-      </c>
-      <c r="AD1" s="45"/>
-      <c r="AE1" s="45"/>
-      <c r="AF1" s="45"/>
-      <c r="AG1" s="45"/>
-      <c r="AH1" s="45"/>
-      <c r="AI1" s="45"/>
-      <c r="AJ1" s="45"/>
+      <c r="AC1" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD1" s="34"/>
+      <c r="AE1" s="34"/>
+      <c r="AF1" s="34"/>
+      <c r="AG1" s="34"/>
+      <c r="AH1" s="34"/>
+      <c r="AI1" s="34"/>
+      <c r="AJ1" s="34"/>
       <c r="AK1" s="35" t="s">
         <v>4</v>
       </c>
@@ -3092,7 +3089,7 @@
       <c r="B2" s="35"/>
       <c r="C2" s="35"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="34"/>
+      <c r="E2" s="38"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -3159,7 +3156,7 @@
       <c r="B3" s="35"/>
       <c r="C3" s="35"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="34"/>
+      <c r="E3" s="38"/>
       <c r="F3" s="5" t="s">
         <v>14</v>
       </c>
@@ -3282,7 +3279,7 @@
       <c r="B4" s="35"/>
       <c r="C4" s="35"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="34"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -3291,25 +3288,25 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
-      <c r="N4" s="47" t="s">
+      <c r="N4" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="O4" s="47"/>
-      <c r="P4" s="47"/>
-      <c r="Q4" s="47"/>
-      <c r="R4" s="47"/>
-      <c r="S4" s="47"/>
-      <c r="T4" s="47"/>
-      <c r="U4" s="47"/>
-      <c r="V4" s="48" t="s">
+      <c r="O4" s="49"/>
+      <c r="P4" s="49"/>
+      <c r="Q4" s="49"/>
+      <c r="R4" s="49"/>
+      <c r="S4" s="49"/>
+      <c r="T4" s="49"/>
+      <c r="U4" s="49"/>
+      <c r="V4" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="W4" s="48"/>
-      <c r="X4" s="48"/>
-      <c r="Y4" s="48"/>
-      <c r="Z4" s="48"/>
-      <c r="AA4" s="48"/>
-      <c r="AB4" s="48"/>
+      <c r="W4" s="50"/>
+      <c r="X4" s="50"/>
+      <c r="Y4" s="50"/>
+      <c r="Z4" s="50"/>
+      <c r="AA4" s="50"/>
+      <c r="AB4" s="50"/>
       <c r="AC4" s="5"/>
       <c r="AD4" s="5"/>
       <c r="AE4" s="5"/>
@@ -3318,51 +3315,51 @@
       <c r="AH4" s="5"/>
       <c r="AI4" s="5"/>
       <c r="AJ4" s="5"/>
-      <c r="AK4" s="47" t="s">
+      <c r="AK4" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="AL4" s="47"/>
-      <c r="AM4" s="47"/>
-      <c r="AN4" s="47"/>
-      <c r="AO4" s="47"/>
-      <c r="AP4" s="47"/>
-      <c r="AQ4" s="47"/>
-      <c r="AR4" s="47"/>
-      <c r="AS4" s="48" t="s">
+      <c r="AL4" s="49"/>
+      <c r="AM4" s="49"/>
+      <c r="AN4" s="49"/>
+      <c r="AO4" s="49"/>
+      <c r="AP4" s="49"/>
+      <c r="AQ4" s="49"/>
+      <c r="AR4" s="49"/>
+      <c r="AS4" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="AT4" s="48"/>
-      <c r="AU4" s="48"/>
-      <c r="AV4" s="48"/>
-      <c r="AW4" s="48"/>
-      <c r="AX4" s="48"/>
-      <c r="AY4" s="48"/>
+      <c r="AT4" s="50"/>
+      <c r="AU4" s="50"/>
+      <c r="AV4" s="50"/>
+      <c r="AW4" s="50"/>
+      <c r="AX4" s="50"/>
+      <c r="AY4" s="50"/>
       <c r="AZ4" s="7"/>
       <c r="BA4" s="7"/>
-      <c r="BB4" s="44" t="s">
+      <c r="BB4" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="BC4" s="44"/>
+      <c r="BC4" s="32"/>
       <c r="BD4" s="4"/>
       <c r="BE4" s="4"/>
-      <c r="BF4" s="41" t="s">
-        <v>100</v>
-      </c>
-      <c r="BG4" s="42"/>
-      <c r="BH4" s="42"/>
-      <c r="BI4" s="42"/>
-      <c r="BJ4" s="42"/>
-      <c r="BK4" s="42"/>
-      <c r="BL4" s="42"/>
-      <c r="BM4" s="42"/>
-      <c r="BN4" s="42"/>
-      <c r="BO4" s="42"/>
-      <c r="BP4" s="42"/>
-      <c r="BQ4" s="42"/>
-      <c r="BR4" s="42"/>
-      <c r="BS4" s="42"/>
-      <c r="BT4" s="32" t="s">
-        <v>129</v>
+      <c r="BF4" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="BG4" s="43"/>
+      <c r="BH4" s="43"/>
+      <c r="BI4" s="43"/>
+      <c r="BJ4" s="43"/>
+      <c r="BK4" s="43"/>
+      <c r="BL4" s="43"/>
+      <c r="BM4" s="43"/>
+      <c r="BN4" s="43"/>
+      <c r="BO4" s="43"/>
+      <c r="BP4" s="43"/>
+      <c r="BQ4" s="43"/>
+      <c r="BR4" s="43"/>
+      <c r="BS4" s="43"/>
+      <c r="BT4" s="37" t="s">
+        <v>112</v>
       </c>
       <c r="BU4" s="33"/>
       <c r="BV4" s="33"/>
@@ -3385,7 +3382,7 @@
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="15" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="5">
@@ -3539,265 +3536,260 @@
         <v>32</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>33</v>
       </c>
       <c r="F6" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="P6" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q6" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="R6" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="S6" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="T6" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="U6" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="V6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="W6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="X6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="Y6" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="Z6" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="AA6" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="AB6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="M6" s="11" t="s">
+      <c r="AC6" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="AD6" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="AE6" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="P6" s="11" t="s">
+      <c r="AF6" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="Q6" s="11" t="s">
+      <c r="AG6" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="R6" s="11" t="s">
+      <c r="AH6" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="S6" s="11" t="s">
+      <c r="AI6" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="T6" s="11" t="s">
+      <c r="AJ6" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="U6" s="11" t="s">
+      <c r="AK6" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="V6" s="11" t="s">
+      <c r="AL6" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="W6" s="11" t="s">
+      <c r="AM6" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="X6" s="11" t="s">
+      <c r="AN6" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="Y6" s="11" t="s">
+      <c r="AO6" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="Z6" s="11" t="s">
+      <c r="AP6" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="AA6" s="11" t="s">
+      <c r="AQ6" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="AB6" s="11" t="s">
+      <c r="AR6" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AC6" s="11" t="s">
+      <c r="AS6" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="AD6" s="11" t="s">
+      <c r="AT6" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="AE6" s="11" t="s">
+      <c r="AU6" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="AF6" s="11" t="s">
+      <c r="AV6" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AG6" s="11" t="s">
+      <c r="AW6" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AH6" s="11" t="s">
+      <c r="AX6" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="AI6" s="11" t="s">
+      <c r="AY6" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="AJ6" s="11" t="s">
+      <c r="AZ6" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="AK6" s="11" t="s">
+      <c r="BA6" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="AL6" s="11" t="s">
+      <c r="BB6" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="AM6" s="11" t="s">
+      <c r="BC6" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="AN6" s="11" t="s">
+      <c r="BD6" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="AO6" s="11" t="s">
+      <c r="BE6" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="AP6" s="11" t="s">
+      <c r="BF6" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="AQ6" s="11" t="s">
+      <c r="BG6" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="AR6" s="11" t="s">
+      <c r="BH6" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="AS6" s="11" t="s">
+      <c r="BI6" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="AT6" s="11" t="s">
+      <c r="BJ6" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="AU6" s="11" t="s">
+      <c r="BK6" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="AV6" s="11" t="s">
+      <c r="BL6" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="AW6" s="11" t="s">
+      <c r="BM6" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="AX6" s="11" t="s">
+      <c r="BN6" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="AY6" s="11" t="s">
+      <c r="BO6" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="AZ6" s="11" t="s">
+      <c r="BP6" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="BA6" s="11" t="s">
+      <c r="BQ6" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="BB6" s="11" t="s">
+      <c r="BR6" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="BC6" s="11" t="s">
+      <c r="BS6" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="BD6" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="BE6" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="BF6" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="BG6" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="BH6" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="BI6" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="BJ6" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="BK6" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL6" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="BM6" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="BN6" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="BO6" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="BP6" s="14" t="s">
+      <c r="BT6" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="BQ6" s="14" t="s">
+      <c r="BU6" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="BR6" s="13" t="s">
+      <c r="BV6" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="BS6" s="13" t="s">
+      <c r="BW6" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="BT6" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="BU6" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="BV6" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="BW6" s="25" t="s">
-        <v>116</v>
-      </c>
       <c r="BX6" s="25" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="BY6" s="25" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="BZ6" s="25" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="CA6" s="25" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="CB6" s="24" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="CC6" s="14" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="CD6" s="14" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="CE6" s="14" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="CF6" s="14" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="CG6" s="14" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="CH6" s="14" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="CI6" s="14" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="N4:U4"/>
-    <mergeCell ref="V4:AB4"/>
-    <mergeCell ref="AK4:AR4"/>
-    <mergeCell ref="AS4:AY4"/>
-    <mergeCell ref="E1:E4"/>
     <mergeCell ref="BT4:CI4"/>
     <mergeCell ref="C1:C4"/>
     <mergeCell ref="B1:B4"/>
@@ -3813,6 +3805,11 @@
     <mergeCell ref="V2:AB2"/>
     <mergeCell ref="AK2:AR2"/>
     <mergeCell ref="AS2:AY2"/>
+    <mergeCell ref="N4:U4"/>
+    <mergeCell ref="V4:AB4"/>
+    <mergeCell ref="AK4:AR4"/>
+    <mergeCell ref="AS4:AY4"/>
+    <mergeCell ref="E1:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3835,7 +3832,7 @@
   <sheetData>
     <row r="4" spans="3:18" ht="15.75" customHeight="1">
       <c r="C4" s="51" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="D4" s="51"/>
       <c r="E4" s="51"/>
@@ -3871,52 +3868,52 @@
     </row>
     <row r="6" spans="3:18" ht="45">
       <c r="C6" s="14" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="M6" s="14" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="N6" s="14" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="O6" s="14" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="P6" s="14" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="Q6" s="13" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="R6" s="13" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -3932,8 +3929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CI6"/>
   <sheetViews>
-    <sheetView topLeftCell="BB1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="CD3" sqref="CD3:CE3"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6:U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1"/>
@@ -3947,26 +3944,26 @@
   <sheetData>
     <row r="1" spans="1:87" ht="75" customHeight="1">
       <c r="A1" s="2"/>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="47" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="35" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2"/>
-      <c r="E1" s="34" t="s">
-        <v>105</v>
-      </c>
-      <c r="F1" s="50" t="s">
-        <v>101</v>
-      </c>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
+      <c r="E1" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
       <c r="N1" s="35" t="s">
         <v>2</v>
       </c>
@@ -3986,16 +3983,16 @@
       <c r="Z1" s="35"/>
       <c r="AA1" s="35"/>
       <c r="AB1" s="35"/>
-      <c r="AC1" s="45" t="s">
-        <v>135</v>
-      </c>
-      <c r="AD1" s="45"/>
-      <c r="AE1" s="45"/>
-      <c r="AF1" s="45"/>
-      <c r="AG1" s="45"/>
-      <c r="AH1" s="45"/>
-      <c r="AI1" s="45"/>
-      <c r="AJ1" s="45"/>
+      <c r="AC1" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD1" s="34"/>
+      <c r="AE1" s="34"/>
+      <c r="AF1" s="34"/>
+      <c r="AG1" s="34"/>
+      <c r="AH1" s="34"/>
+      <c r="AI1" s="34"/>
+      <c r="AJ1" s="34"/>
       <c r="AK1" s="35" t="s">
         <v>4</v>
       </c>
@@ -4036,20 +4033,20 @@
     </row>
     <row r="2" spans="1:87">
       <c r="A2" s="2"/>
-      <c r="B2" s="49"/>
+      <c r="B2" s="47"/>
       <c r="C2" s="35"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="36" t="s">
-        <v>110</v>
-      </c>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="41"/>
       <c r="N2" s="35" t="s">
         <v>11</v>
       </c>
@@ -4069,16 +4066,16 @@
       <c r="Z2" s="35"/>
       <c r="AA2" s="35"/>
       <c r="AB2" s="35"/>
-      <c r="AC2" s="36" t="s">
-        <v>110</v>
-      </c>
-      <c r="AD2" s="37"/>
-      <c r="AE2" s="37"/>
-      <c r="AF2" s="37"/>
-      <c r="AG2" s="37"/>
-      <c r="AH2" s="37"/>
-      <c r="AI2" s="37"/>
-      <c r="AJ2" s="38"/>
+      <c r="AC2" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="AD2" s="40"/>
+      <c r="AE2" s="40"/>
+      <c r="AF2" s="40"/>
+      <c r="AG2" s="40"/>
+      <c r="AH2" s="40"/>
+      <c r="AI2" s="40"/>
+      <c r="AJ2" s="41"/>
       <c r="AK2" s="35" t="s">
         <v>13</v>
       </c>
@@ -4104,34 +4101,34 @@
       <c r="BC2" s="35"/>
       <c r="BD2" s="4"/>
       <c r="BE2" s="4"/>
-      <c r="CB2" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="CC2" s="30"/>
-      <c r="CD2" s="30"/>
-      <c r="CE2" s="30"/>
-      <c r="CF2" s="30"/>
-      <c r="CG2" s="30"/>
-      <c r="CH2" s="30"/>
-      <c r="CI2" s="30"/>
+      <c r="CB2" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="CC2" s="45"/>
+      <c r="CD2" s="45"/>
+      <c r="CE2" s="45"/>
+      <c r="CF2" s="45"/>
+      <c r="CG2" s="45"/>
+      <c r="CH2" s="45"/>
+      <c r="CI2" s="45"/>
     </row>
     <row r="3" spans="1:87" ht="30.75" customHeight="1" thickBot="1">
       <c r="A3" s="2"/>
-      <c r="B3" s="49"/>
+      <c r="B3" s="47"/>
       <c r="C3" s="35"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="34"/>
+      <c r="E3" s="38"/>
       <c r="F3" s="5" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>16</v>
@@ -4146,16 +4143,16 @@
         <v>19</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="R3" s="5" t="s">
         <v>16</v>
@@ -4177,16 +4174,16 @@
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
       <c r="AC3" s="5" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="AD3" s="5" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="AE3" s="5" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="AF3" s="5" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="AG3" s="5" t="s">
         <v>16</v>
@@ -4201,16 +4198,16 @@
         <v>19</v>
       </c>
       <c r="AK3" s="5" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="AL3" s="5" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="AM3" s="5" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="AN3" s="5" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="AO3" s="5" t="s">
         <v>16</v>
@@ -4237,45 +4234,45 @@
       <c r="BC3" s="35"/>
       <c r="BD3" s="4"/>
       <c r="BE3" s="4"/>
-      <c r="BT3" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="BU3" s="31"/>
-      <c r="BV3" s="53" t="s">
-        <v>131</v>
-      </c>
-      <c r="BW3" s="53"/>
-      <c r="BX3" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="BY3" s="31"/>
-      <c r="BZ3" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="CA3" s="31"/>
-      <c r="CB3" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="CC3" s="31"/>
-      <c r="CD3" s="53" t="s">
-        <v>131</v>
-      </c>
-      <c r="CE3" s="53"/>
-      <c r="CF3" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="CG3" s="31"/>
-      <c r="CH3" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="CI3" s="31"/>
+      <c r="BT3" s="46" t="s">
+        <v>113</v>
+      </c>
+      <c r="BU3" s="46"/>
+      <c r="BV3" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="BW3" s="54"/>
+      <c r="BX3" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="BY3" s="46"/>
+      <c r="BZ3" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="CA3" s="46"/>
+      <c r="CB3" s="46" t="s">
+        <v>113</v>
+      </c>
+      <c r="CC3" s="46"/>
+      <c r="CD3" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="CE3" s="54"/>
+      <c r="CF3" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="CG3" s="46"/>
+      <c r="CH3" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="CI3" s="46"/>
     </row>
     <row r="4" spans="1:87" ht="35.25" customHeight="1" thickBot="1">
       <c r="A4" s="2"/>
-      <c r="B4" s="49"/>
+      <c r="B4" s="47"/>
       <c r="C4" s="35"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="34"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -4284,25 +4281,25 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
-      <c r="N4" s="47" t="s">
+      <c r="N4" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="O4" s="47"/>
-      <c r="P4" s="47"/>
-      <c r="Q4" s="47"/>
-      <c r="R4" s="47"/>
-      <c r="S4" s="47"/>
-      <c r="T4" s="47"/>
-      <c r="U4" s="47"/>
-      <c r="V4" s="48" t="s">
+      <c r="O4" s="49"/>
+      <c r="P4" s="49"/>
+      <c r="Q4" s="49"/>
+      <c r="R4" s="49"/>
+      <c r="S4" s="49"/>
+      <c r="T4" s="49"/>
+      <c r="U4" s="49"/>
+      <c r="V4" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="W4" s="48"/>
-      <c r="X4" s="48"/>
-      <c r="Y4" s="48"/>
-      <c r="Z4" s="48"/>
-      <c r="AA4" s="48"/>
-      <c r="AB4" s="48"/>
+      <c r="W4" s="50"/>
+      <c r="X4" s="50"/>
+      <c r="Y4" s="50"/>
+      <c r="Z4" s="50"/>
+      <c r="AA4" s="50"/>
+      <c r="AB4" s="50"/>
       <c r="AC4" s="5"/>
       <c r="AD4" s="5"/>
       <c r="AE4" s="5"/>
@@ -4311,51 +4308,51 @@
       <c r="AH4" s="5"/>
       <c r="AI4" s="5"/>
       <c r="AJ4" s="5"/>
-      <c r="AK4" s="47" t="s">
+      <c r="AK4" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="AL4" s="47"/>
-      <c r="AM4" s="47"/>
-      <c r="AN4" s="47"/>
-      <c r="AO4" s="47"/>
-      <c r="AP4" s="47"/>
-      <c r="AQ4" s="47"/>
-      <c r="AR4" s="47"/>
-      <c r="AS4" s="48" t="s">
+      <c r="AL4" s="49"/>
+      <c r="AM4" s="49"/>
+      <c r="AN4" s="49"/>
+      <c r="AO4" s="49"/>
+      <c r="AP4" s="49"/>
+      <c r="AQ4" s="49"/>
+      <c r="AR4" s="49"/>
+      <c r="AS4" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="AT4" s="48"/>
-      <c r="AU4" s="48"/>
-      <c r="AV4" s="48"/>
-      <c r="AW4" s="48"/>
-      <c r="AX4" s="48"/>
-      <c r="AY4" s="48"/>
+      <c r="AT4" s="50"/>
+      <c r="AU4" s="50"/>
+      <c r="AV4" s="50"/>
+      <c r="AW4" s="50"/>
+      <c r="AX4" s="50"/>
+      <c r="AY4" s="50"/>
       <c r="AZ4" s="7"/>
       <c r="BA4" s="7"/>
-      <c r="BB4" s="44" t="s">
+      <c r="BB4" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="BC4" s="44"/>
+      <c r="BC4" s="32"/>
       <c r="BD4" s="4"/>
       <c r="BE4" s="4"/>
-      <c r="BF4" s="41" t="s">
-        <v>100</v>
-      </c>
-      <c r="BG4" s="42"/>
-      <c r="BH4" s="42"/>
-      <c r="BI4" s="42"/>
-      <c r="BJ4" s="42"/>
-      <c r="BK4" s="42"/>
-      <c r="BL4" s="42"/>
-      <c r="BM4" s="42"/>
-      <c r="BN4" s="42"/>
-      <c r="BO4" s="42"/>
-      <c r="BP4" s="42"/>
-      <c r="BQ4" s="42"/>
-      <c r="BR4" s="42"/>
-      <c r="BS4" s="54"/>
-      <c r="BT4" s="32" t="s">
-        <v>129</v>
+      <c r="BF4" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="BG4" s="43"/>
+      <c r="BH4" s="43"/>
+      <c r="BI4" s="43"/>
+      <c r="BJ4" s="43"/>
+      <c r="BK4" s="43"/>
+      <c r="BL4" s="43"/>
+      <c r="BM4" s="43"/>
+      <c r="BN4" s="43"/>
+      <c r="BO4" s="43"/>
+      <c r="BP4" s="43"/>
+      <c r="BQ4" s="43"/>
+      <c r="BR4" s="43"/>
+      <c r="BS4" s="53"/>
+      <c r="BT4" s="37" t="s">
+        <v>112</v>
       </c>
       <c r="BU4" s="33"/>
       <c r="BV4" s="33"/>
@@ -4378,7 +4375,7 @@
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="21" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="5">
@@ -4532,275 +4529,269 @@
         <v>32</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>33</v>
       </c>
       <c r="F6" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="P6" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q6" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="R6" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="S6" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="T6" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="U6" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="V6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="W6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="X6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="Y6" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="Z6" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="AA6" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="AB6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="M6" s="11" t="s">
+      <c r="AC6" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="AD6" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="AE6" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="P6" s="11" t="s">
+      <c r="AF6" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="Q6" s="11" t="s">
+      <c r="AG6" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="R6" s="11" t="s">
+      <c r="AH6" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="S6" s="11" t="s">
+      <c r="AI6" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="T6" s="11" t="s">
+      <c r="AJ6" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="U6" s="11" t="s">
+      <c r="AK6" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="V6" s="11" t="s">
+      <c r="AL6" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="W6" s="11" t="s">
+      <c r="AM6" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="X6" s="11" t="s">
+      <c r="AN6" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="Y6" s="11" t="s">
+      <c r="AO6" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="Z6" s="11" t="s">
+      <c r="AP6" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="AA6" s="11" t="s">
+      <c r="AQ6" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="AB6" s="11" t="s">
+      <c r="AR6" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AC6" s="11" t="s">
+      <c r="AS6" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="AD6" s="11" t="s">
+      <c r="AT6" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="AE6" s="11" t="s">
+      <c r="AU6" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="AF6" s="11" t="s">
+      <c r="AV6" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AG6" s="11" t="s">
+      <c r="AW6" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AH6" s="11" t="s">
+      <c r="AX6" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="AI6" s="11" t="s">
+      <c r="AY6" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="AJ6" s="11" t="s">
+      <c r="AZ6" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="AK6" s="11" t="s">
+      <c r="BA6" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="AL6" s="11" t="s">
+      <c r="BB6" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="AM6" s="11" t="s">
+      <c r="BC6" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="AN6" s="11" t="s">
+      <c r="BD6" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="AO6" s="11" t="s">
+      <c r="BE6" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="AP6" s="11" t="s">
+      <c r="BF6" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="AQ6" s="11" t="s">
+      <c r="BG6" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="AR6" s="11" t="s">
+      <c r="BH6" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="AS6" s="11" t="s">
+      <c r="BI6" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="AT6" s="11" t="s">
+      <c r="BJ6" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="AU6" s="11" t="s">
+      <c r="BK6" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="AV6" s="11" t="s">
+      <c r="BL6" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="AW6" s="11" t="s">
+      <c r="BM6" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="AX6" s="11" t="s">
+      <c r="BN6" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="AY6" s="11" t="s">
+      <c r="BO6" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="AZ6" s="11" t="s">
+      <c r="BP6" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="BA6" s="11" t="s">
+      <c r="BQ6" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="BB6" s="11" t="s">
+      <c r="BR6" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="BC6" s="11" t="s">
+      <c r="BS6" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="BD6" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="BE6" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="BF6" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="BG6" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="BH6" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="BI6" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="BJ6" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="BK6" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL6" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="BM6" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="BN6" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="BO6" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="BP6" s="14" t="s">
+      <c r="BT6" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="BQ6" s="14" t="s">
+      <c r="BU6" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="BR6" s="13" t="s">
+      <c r="BV6" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="BS6" s="13" t="s">
+      <c r="BW6" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="BT6" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="BU6" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="BV6" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="BW6" s="25" t="s">
-        <v>116</v>
-      </c>
       <c r="BX6" s="25" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="BY6" s="25" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="BZ6" s="25" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="CA6" s="25" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="CB6" s="24" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="CC6" s="14" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="CD6" s="14" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="CE6" s="14" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="CF6" s="14" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="CG6" s="14" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="CH6" s="14" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="CI6" s="14" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="BT4:CI4"/>
-    <mergeCell ref="AK4:AR4"/>
-    <mergeCell ref="AS4:AY4"/>
-    <mergeCell ref="BB4:BC4"/>
-    <mergeCell ref="BF4:BS4"/>
-    <mergeCell ref="BC1:BC3"/>
-    <mergeCell ref="AS2:AY2"/>
-    <mergeCell ref="BB1:BB3"/>
-    <mergeCell ref="AC1:AJ1"/>
-    <mergeCell ref="AK1:AR1"/>
-    <mergeCell ref="AS1:AY1"/>
-    <mergeCell ref="AZ1:AZ3"/>
-    <mergeCell ref="BA1:BA3"/>
-    <mergeCell ref="AC2:AJ2"/>
-    <mergeCell ref="AK2:AR2"/>
+    <mergeCell ref="CB2:CI2"/>
+    <mergeCell ref="BT3:BU3"/>
+    <mergeCell ref="BV3:BW3"/>
+    <mergeCell ref="BX3:BY3"/>
+    <mergeCell ref="BZ3:CA3"/>
+    <mergeCell ref="CB3:CC3"/>
+    <mergeCell ref="CD3:CE3"/>
+    <mergeCell ref="CF3:CG3"/>
+    <mergeCell ref="CH3:CI3"/>
     <mergeCell ref="V1:AB1"/>
     <mergeCell ref="N4:U4"/>
     <mergeCell ref="V4:AB4"/>
@@ -4812,15 +4803,21 @@
     <mergeCell ref="F2:M2"/>
     <mergeCell ref="N2:U2"/>
     <mergeCell ref="V2:AB2"/>
-    <mergeCell ref="CB2:CI2"/>
-    <mergeCell ref="BT3:BU3"/>
-    <mergeCell ref="BV3:BW3"/>
-    <mergeCell ref="BX3:BY3"/>
-    <mergeCell ref="BZ3:CA3"/>
-    <mergeCell ref="CB3:CC3"/>
-    <mergeCell ref="CD3:CE3"/>
-    <mergeCell ref="CF3:CG3"/>
-    <mergeCell ref="CH3:CI3"/>
+    <mergeCell ref="BC1:BC3"/>
+    <mergeCell ref="AS2:AY2"/>
+    <mergeCell ref="BB1:BB3"/>
+    <mergeCell ref="AC1:AJ1"/>
+    <mergeCell ref="AK1:AR1"/>
+    <mergeCell ref="AS1:AY1"/>
+    <mergeCell ref="AZ1:AZ3"/>
+    <mergeCell ref="BA1:BA3"/>
+    <mergeCell ref="AC2:AJ2"/>
+    <mergeCell ref="AK2:AR2"/>
+    <mergeCell ref="BT4:CI4"/>
+    <mergeCell ref="AK4:AR4"/>
+    <mergeCell ref="AS4:AY4"/>
+    <mergeCell ref="BB4:BC4"/>
+    <mergeCell ref="BF4:BS4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4831,7 +4828,7 @@
   <dimension ref="A1:CI6"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1"/>
@@ -4845,26 +4842,26 @@
   <sheetData>
     <row r="1" spans="1:87" ht="75" customHeight="1">
       <c r="A1" s="2"/>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="47" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="35" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2"/>
-      <c r="E1" s="34" t="s">
-        <v>105</v>
-      </c>
-      <c r="F1" s="50" t="s">
-        <v>101</v>
-      </c>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
+      <c r="E1" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
       <c r="N1" s="35" t="s">
         <v>2</v>
       </c>
@@ -4884,16 +4881,16 @@
       <c r="Z1" s="35"/>
       <c r="AA1" s="35"/>
       <c r="AB1" s="35"/>
-      <c r="AC1" s="45" t="s">
-        <v>135</v>
-      </c>
-      <c r="AD1" s="45"/>
-      <c r="AE1" s="45"/>
-      <c r="AF1" s="45"/>
-      <c r="AG1" s="45"/>
-      <c r="AH1" s="45"/>
-      <c r="AI1" s="45"/>
-      <c r="AJ1" s="45"/>
+      <c r="AC1" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD1" s="34"/>
+      <c r="AE1" s="34"/>
+      <c r="AF1" s="34"/>
+      <c r="AG1" s="34"/>
+      <c r="AH1" s="34"/>
+      <c r="AI1" s="34"/>
+      <c r="AJ1" s="34"/>
       <c r="AK1" s="35" t="s">
         <v>4</v>
       </c>
@@ -4932,22 +4929,22 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:87">
+    <row r="2" spans="1:87" ht="15" customHeight="1">
       <c r="A2" s="2"/>
-      <c r="B2" s="49"/>
+      <c r="B2" s="47"/>
       <c r="C2" s="35"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="36" t="s">
-        <v>110</v>
-      </c>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="41"/>
       <c r="N2" s="35" t="s">
         <v>11</v>
       </c>
@@ -4967,16 +4964,16 @@
       <c r="Z2" s="35"/>
       <c r="AA2" s="35"/>
       <c r="AB2" s="35"/>
-      <c r="AC2" s="36" t="s">
-        <v>110</v>
-      </c>
-      <c r="AD2" s="37"/>
-      <c r="AE2" s="37"/>
-      <c r="AF2" s="37"/>
-      <c r="AG2" s="37"/>
-      <c r="AH2" s="37"/>
-      <c r="AI2" s="37"/>
-      <c r="AJ2" s="38"/>
+      <c r="AC2" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="AD2" s="40"/>
+      <c r="AE2" s="40"/>
+      <c r="AF2" s="40"/>
+      <c r="AG2" s="40"/>
+      <c r="AH2" s="40"/>
+      <c r="AI2" s="40"/>
+      <c r="AJ2" s="41"/>
       <c r="AK2" s="35" t="s">
         <v>13</v>
       </c>
@@ -5002,34 +4999,34 @@
       <c r="BC2" s="35"/>
       <c r="BD2" s="4"/>
       <c r="BE2" s="4"/>
-      <c r="CB2" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="CC2" s="30"/>
-      <c r="CD2" s="30"/>
-      <c r="CE2" s="30"/>
-      <c r="CF2" s="30"/>
-      <c r="CG2" s="30"/>
-      <c r="CH2" s="30"/>
-      <c r="CI2" s="30"/>
+      <c r="CB2" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="CC2" s="45"/>
+      <c r="CD2" s="45"/>
+      <c r="CE2" s="45"/>
+      <c r="CF2" s="45"/>
+      <c r="CG2" s="45"/>
+      <c r="CH2" s="45"/>
+      <c r="CI2" s="45"/>
     </row>
     <row r="3" spans="1:87" ht="30.75" customHeight="1" thickBot="1">
       <c r="A3" s="2"/>
-      <c r="B3" s="49"/>
+      <c r="B3" s="47"/>
       <c r="C3" s="35"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="34"/>
+      <c r="E3" s="38"/>
       <c r="F3" s="5" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>16</v>
@@ -5044,16 +5041,16 @@
         <v>19</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="R3" s="5" t="s">
         <v>16</v>
@@ -5067,24 +5064,24 @@
       <c r="U3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
-      <c r="AA3" s="2"/>
-      <c r="AB3" s="2"/>
+      <c r="V3" s="35"/>
+      <c r="W3" s="35"/>
+      <c r="X3" s="35"/>
+      <c r="Y3" s="35"/>
+      <c r="Z3" s="35"/>
+      <c r="AA3" s="35"/>
+      <c r="AB3" s="35"/>
       <c r="AC3" s="5" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="AD3" s="5" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="AE3" s="5" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="AF3" s="5" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="AG3" s="5" t="s">
         <v>16</v>
@@ -5099,16 +5096,16 @@
         <v>19</v>
       </c>
       <c r="AK3" s="5" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="AL3" s="5" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="AM3" s="5" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="AN3" s="5" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="AO3" s="5" t="s">
         <v>16</v>
@@ -5135,45 +5132,45 @@
       <c r="BC3" s="35"/>
       <c r="BD3" s="4"/>
       <c r="BE3" s="4"/>
-      <c r="BT3" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="BU3" s="31"/>
-      <c r="BV3" s="53" t="s">
-        <v>131</v>
-      </c>
-      <c r="BW3" s="53"/>
-      <c r="BX3" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="BY3" s="31"/>
-      <c r="BZ3" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="CA3" s="31"/>
-      <c r="CB3" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="CC3" s="31"/>
-      <c r="CD3" s="53" t="s">
-        <v>131</v>
-      </c>
-      <c r="CE3" s="53"/>
-      <c r="CF3" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="CG3" s="31"/>
-      <c r="CH3" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="CI3" s="31"/>
+      <c r="BT3" s="46" t="s">
+        <v>113</v>
+      </c>
+      <c r="BU3" s="46"/>
+      <c r="BV3" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="BW3" s="54"/>
+      <c r="BX3" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="BY3" s="46"/>
+      <c r="BZ3" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="CA3" s="46"/>
+      <c r="CB3" s="46" t="s">
+        <v>113</v>
+      </c>
+      <c r="CC3" s="46"/>
+      <c r="CD3" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="CE3" s="54"/>
+      <c r="CF3" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="CG3" s="46"/>
+      <c r="CH3" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="CI3" s="46"/>
     </row>
     <row r="4" spans="1:87" ht="35.25" customHeight="1" thickBot="1">
       <c r="A4" s="2"/>
-      <c r="B4" s="49"/>
+      <c r="B4" s="47"/>
       <c r="C4" s="35"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="34"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -5182,25 +5179,25 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
-      <c r="N4" s="47" t="s">
+      <c r="N4" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="O4" s="47"/>
-      <c r="P4" s="47"/>
-      <c r="Q4" s="47"/>
-      <c r="R4" s="47"/>
-      <c r="S4" s="47"/>
-      <c r="T4" s="47"/>
-      <c r="U4" s="47"/>
-      <c r="V4" s="48" t="s">
+      <c r="O4" s="49"/>
+      <c r="P4" s="49"/>
+      <c r="Q4" s="49"/>
+      <c r="R4" s="49"/>
+      <c r="S4" s="49"/>
+      <c r="T4" s="49"/>
+      <c r="U4" s="49"/>
+      <c r="V4" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="W4" s="48"/>
-      <c r="X4" s="48"/>
-      <c r="Y4" s="48"/>
-      <c r="Z4" s="48"/>
-      <c r="AA4" s="48"/>
-      <c r="AB4" s="48"/>
+      <c r="W4" s="50"/>
+      <c r="X4" s="50"/>
+      <c r="Y4" s="50"/>
+      <c r="Z4" s="50"/>
+      <c r="AA4" s="50"/>
+      <c r="AB4" s="50"/>
       <c r="AC4" s="5"/>
       <c r="AD4" s="5"/>
       <c r="AE4" s="5"/>
@@ -5209,51 +5206,51 @@
       <c r="AH4" s="5"/>
       <c r="AI4" s="5"/>
       <c r="AJ4" s="5"/>
-      <c r="AK4" s="47" t="s">
+      <c r="AK4" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="AL4" s="47"/>
-      <c r="AM4" s="47"/>
-      <c r="AN4" s="47"/>
-      <c r="AO4" s="47"/>
-      <c r="AP4" s="47"/>
-      <c r="AQ4" s="47"/>
-      <c r="AR4" s="47"/>
-      <c r="AS4" s="48" t="s">
+      <c r="AL4" s="49"/>
+      <c r="AM4" s="49"/>
+      <c r="AN4" s="49"/>
+      <c r="AO4" s="49"/>
+      <c r="AP4" s="49"/>
+      <c r="AQ4" s="49"/>
+      <c r="AR4" s="49"/>
+      <c r="AS4" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="AT4" s="48"/>
-      <c r="AU4" s="48"/>
-      <c r="AV4" s="48"/>
-      <c r="AW4" s="48"/>
-      <c r="AX4" s="48"/>
-      <c r="AY4" s="48"/>
+      <c r="AT4" s="50"/>
+      <c r="AU4" s="50"/>
+      <c r="AV4" s="50"/>
+      <c r="AW4" s="50"/>
+      <c r="AX4" s="50"/>
+      <c r="AY4" s="50"/>
       <c r="AZ4" s="7"/>
       <c r="BA4" s="7"/>
-      <c r="BB4" s="44" t="s">
+      <c r="BB4" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="BC4" s="44"/>
+      <c r="BC4" s="32"/>
       <c r="BD4" s="4"/>
       <c r="BE4" s="4"/>
-      <c r="BF4" s="41" t="s">
-        <v>100</v>
-      </c>
-      <c r="BG4" s="42"/>
-      <c r="BH4" s="42"/>
-      <c r="BI4" s="42"/>
-      <c r="BJ4" s="42"/>
-      <c r="BK4" s="42"/>
-      <c r="BL4" s="42"/>
-      <c r="BM4" s="42"/>
-      <c r="BN4" s="42"/>
-      <c r="BO4" s="42"/>
-      <c r="BP4" s="42"/>
-      <c r="BQ4" s="42"/>
-      <c r="BR4" s="42"/>
-      <c r="BS4" s="54"/>
-      <c r="BT4" s="32" t="s">
-        <v>129</v>
+      <c r="BF4" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="BG4" s="43"/>
+      <c r="BH4" s="43"/>
+      <c r="BI4" s="43"/>
+      <c r="BJ4" s="43"/>
+      <c r="BK4" s="43"/>
+      <c r="BL4" s="43"/>
+      <c r="BM4" s="43"/>
+      <c r="BN4" s="43"/>
+      <c r="BO4" s="43"/>
+      <c r="BP4" s="43"/>
+      <c r="BQ4" s="43"/>
+      <c r="BR4" s="43"/>
+      <c r="BS4" s="53"/>
+      <c r="BT4" s="37" t="s">
+        <v>112</v>
       </c>
       <c r="BU4" s="33"/>
       <c r="BV4" s="33"/>
@@ -5276,7 +5273,7 @@
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="27" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="5">
@@ -5430,271 +5427,277 @@
         <v>32</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>33</v>
       </c>
       <c r="F6" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="O6" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="P6" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q6" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="R6" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="S6" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="T6" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="U6" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="V6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="W6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="X6" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="Y6" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="Z6" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="AA6" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="AB6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="M6" s="11" t="s">
+      <c r="AC6" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="AD6" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="AE6" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="P6" s="11" t="s">
+      <c r="AF6" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="Q6" s="11" t="s">
+      <c r="AG6" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="R6" s="11" t="s">
+      <c r="AH6" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="S6" s="11" t="s">
+      <c r="AI6" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="T6" s="11" t="s">
+      <c r="AJ6" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="U6" s="11" t="s">
+      <c r="AK6" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="V6" s="11" t="s">
+      <c r="AL6" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="W6" s="11" t="s">
+      <c r="AM6" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="X6" s="11" t="s">
+      <c r="AN6" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="Y6" s="11" t="s">
+      <c r="AO6" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="Z6" s="11" t="s">
+      <c r="AP6" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="AA6" s="11" t="s">
+      <c r="AQ6" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="AB6" s="11" t="s">
+      <c r="AR6" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AC6" s="11" t="s">
+      <c r="AS6" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="AD6" s="11" t="s">
+      <c r="AT6" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="AE6" s="11" t="s">
+      <c r="AU6" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="AF6" s="11" t="s">
+      <c r="AV6" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AG6" s="11" t="s">
+      <c r="AW6" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AH6" s="11" t="s">
+      <c r="AX6" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="AI6" s="11" t="s">
+      <c r="AY6" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="AJ6" s="11" t="s">
+      <c r="AZ6" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="AK6" s="11" t="s">
+      <c r="BA6" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="AL6" s="11" t="s">
+      <c r="BB6" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="AM6" s="11" t="s">
+      <c r="BC6" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="AN6" s="11" t="s">
+      <c r="BD6" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="AO6" s="11" t="s">
+      <c r="BE6" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="AP6" s="11" t="s">
+      <c r="BF6" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="AQ6" s="11" t="s">
+      <c r="BG6" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="AR6" s="11" t="s">
+      <c r="BH6" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="AS6" s="11" t="s">
+      <c r="BI6" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="AT6" s="11" t="s">
+      <c r="BJ6" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="AU6" s="11" t="s">
+      <c r="BK6" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="AV6" s="11" t="s">
+      <c r="BL6" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="AW6" s="11" t="s">
+      <c r="BM6" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="AX6" s="11" t="s">
+      <c r="BN6" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="AY6" s="11" t="s">
+      <c r="BO6" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="AZ6" s="11" t="s">
+      <c r="BP6" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="BA6" s="11" t="s">
+      <c r="BQ6" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="BB6" s="11" t="s">
+      <c r="BR6" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="BC6" s="11" t="s">
+      <c r="BS6" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="BD6" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="BE6" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="BF6" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="BG6" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="BH6" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="BI6" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="BJ6" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="BK6" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="BL6" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="BM6" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="BN6" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="BO6" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="BP6" s="14" t="s">
+      <c r="BT6" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="BQ6" s="14" t="s">
+      <c r="BU6" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="BR6" s="13" t="s">
+      <c r="BV6" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="BS6" s="13" t="s">
+      <c r="BW6" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="BT6" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="BU6" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="BV6" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="BW6" s="25" t="s">
-        <v>116</v>
-      </c>
       <c r="BX6" s="25" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="BY6" s="25" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="BZ6" s="25" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="CA6" s="25" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="CB6" s="24" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="CC6" s="14" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="CD6" s="14" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="CE6" s="14" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="CF6" s="14" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="CG6" s="14" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="CH6" s="14" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="CI6" s="14" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="V4:AB4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="E1:E4"/>
-    <mergeCell ref="F1:M1"/>
-    <mergeCell ref="N1:U1"/>
-    <mergeCell ref="N4:U4"/>
+    <mergeCell ref="AK4:AR4"/>
+    <mergeCell ref="AS4:AY4"/>
+    <mergeCell ref="BB4:BC4"/>
+    <mergeCell ref="BF4:BS4"/>
+    <mergeCell ref="BT4:CI4"/>
+    <mergeCell ref="CB2:CI2"/>
+    <mergeCell ref="BT3:BU3"/>
+    <mergeCell ref="BV3:BW3"/>
+    <mergeCell ref="BX3:BY3"/>
+    <mergeCell ref="BZ3:CA3"/>
+    <mergeCell ref="CB3:CC3"/>
+    <mergeCell ref="CD3:CE3"/>
+    <mergeCell ref="CF3:CG3"/>
+    <mergeCell ref="CH3:CI3"/>
     <mergeCell ref="BC1:BC3"/>
     <mergeCell ref="F2:M2"/>
     <mergeCell ref="N2:U2"/>
-    <mergeCell ref="V2:AB2"/>
     <mergeCell ref="AC2:AJ2"/>
     <mergeCell ref="AK2:AR2"/>
     <mergeCell ref="AS2:AY2"/>
@@ -5705,20 +5708,14 @@
     <mergeCell ref="BA1:BA3"/>
     <mergeCell ref="BB1:BB3"/>
     <mergeCell ref="V1:AB1"/>
-    <mergeCell ref="CB2:CI2"/>
-    <mergeCell ref="BT3:BU3"/>
-    <mergeCell ref="BV3:BW3"/>
-    <mergeCell ref="BX3:BY3"/>
-    <mergeCell ref="BZ3:CA3"/>
-    <mergeCell ref="CB3:CC3"/>
-    <mergeCell ref="CD3:CE3"/>
-    <mergeCell ref="CF3:CG3"/>
-    <mergeCell ref="CH3:CI3"/>
-    <mergeCell ref="AK4:AR4"/>
-    <mergeCell ref="AS4:AY4"/>
-    <mergeCell ref="BB4:BC4"/>
-    <mergeCell ref="BF4:BS4"/>
-    <mergeCell ref="BT4:CI4"/>
+    <mergeCell ref="V2:AB3"/>
+    <mergeCell ref="V4:AB4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="E1:E4"/>
+    <mergeCell ref="F1:M1"/>
+    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="N4:U4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>